<commit_message>
Changes in testng.xml file
</commit_message>
<xml_diff>
--- a/appium/Results/ExcelSheetsFolder/24062025/ExcelResults.xlsx
+++ b/appium/Results/ExcelSheetsFolder/24062025/ExcelResults.xlsx
@@ -11,6 +11,7 @@
     <sheet name="JSTV220_00.00.72.40.CBSPP_24062" sheetId="1" r:id="rId1"/>
     <sheet name="JMSD200A_23.1.11_24062025" sheetId="2" r:id="rId2"/>
     <sheet name="JSTV210_00.00.43.08-AppCert-YTS" r:id="rId6" sheetId="3"/>
+    <sheet name="JHSD200_11.2.28_24062025" r:id="rId7" sheetId="4"/>
   </sheets>
   <calcPr calcId="0"/>
   <oleSize ref="A1:J16"/>
@@ -18,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="33">
   <si>
     <t>DeviceName</t>
   </si>
@@ -114,6 +115,9 @@
   </si>
   <si>
     <t>JSTV210_00.00.43.08-AppCert-YTS-Jun17</t>
+  </si>
+  <si>
+    <t>JHSD200_11.2.28</t>
   </si>
 </sst>
 </file>
@@ -1089,4 +1093,185 @@
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.88671875"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.17578125"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="28.09765625"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.1171875"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.11328125"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="14.10546875"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F5" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="E7" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F7" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="E8" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F8" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>